<commit_message>
Create an ExcelDB class to allow ready an existing table and querying it
  - with documentation
</commit_message>
<xml_diff>
--- a/test/mountains.xlsx
+++ b/test/mountains.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUO/laurent/Documents/SettleNext2/Div 7 Executive/Development/pythonlib/excel_tables/tests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUO/laurent/Documents/SettleNext2/Div 7 Executive/Development/pythonlib/excel_tables/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33ABFA72-BDF6-4346-A91B-8BB958CD7416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E71C417-0572-4248-A674-B79D846D501F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="3160" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="3160" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mountains" sheetId="1" r:id="rId1"/>
+    <sheet name="Cities" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="104">
   <si>
     <t>Name</t>
   </si>
@@ -336,6 +337,15 @@
   </si>
   <si>
     <t>Ascension</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Altitude</t>
   </si>
 </sst>
 </file>
@@ -343,9 +353,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -362,6 +372,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -387,10 +405,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +824,7 @@
       </c>
       <c r="J2">
         <f ca="1">RAND()</f>
-        <v>0.84554083918691247</v>
+        <v>0.19565021213661404</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -837,7 +857,7 @@
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J26" ca="1" si="0">RAND()</f>
-        <v>5.9035483306554282E-3</v>
+        <v>0.22902659152252836</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -870,7 +890,7 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66091254600363036</v>
+        <v>0.75612862889360799</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -903,7 +923,7 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30217577165858733</v>
+        <v>0.42831088973332443</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -936,7 +956,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.58793144996827207</v>
+        <v>0.31605855813917683</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -969,7 +989,7 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99678130097645767</v>
+        <v>9.3402207363452727E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1002,7 +1022,7 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71713020648143744</v>
+        <v>5.8678175358278128E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1035,7 +1055,7 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94445754897536638</v>
+        <v>0.16100919167868266</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1068,7 +1088,7 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44402052816069248</v>
+        <v>0.80138352786999589</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1101,7 +1121,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8807579411543345E-2</v>
+        <v>0.3876381818585598</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1134,7 +1154,7 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5992821358496242</v>
+        <v>0.26427147293054054</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1167,7 +1187,7 @@
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97229280093718484</v>
+        <v>0.26539115703915483</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1200,7 +1220,7 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91475161586742937</v>
+        <v>0.72355580947484599</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1233,7 +1253,7 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22262620192348992</v>
+        <v>0.81626279635791466</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1266,7 +1286,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73570836695317332</v>
+        <v>0.4373928917187988</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1299,7 +1319,7 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22304090034749835</v>
+        <v>0.74774394311773607</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1332,7 +1352,7 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14576187121904349</v>
+        <v>0.43407772494803953</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1365,7 +1385,7 @@
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.46786355428113624</v>
+        <v>0.1832803466713171</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1398,7 +1418,7 @@
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64589864583305689</v>
+        <v>0.6294085854430137</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1431,7 +1451,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56585461485088417</v>
+        <v>0.66240744232541227</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1464,7 +1484,7 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29725076825676489</v>
+        <v>0.23757369634898351</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1497,7 +1517,7 @@
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34845889869804958</v>
+        <v>0.41009419459910623</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1530,7 +1550,7 @@
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8604760040412478</v>
+        <v>0.44959853766447178</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1563,7 +1583,7 @@
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8577474185675791E-2</v>
+        <v>0.26400432961866915</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,14 +1616,142 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79229431023319641</v>
+        <v>0.28256090673261036</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
     <ignoredError sqref="A1 E3:F26 I3:I26 E2:F2 I2 E1:I1 A2:C2 A3:C26" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2179DB8B-1E4D-784B-BA8E-3931701E4811}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1442271</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1324</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4">
+        <v>26023</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2228</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="4">
+        <v>118805</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2045</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4">
+        <v>599504</v>
+      </c>
+      <c r="C5">
+        <v>822</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4">
+        <v>252201</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1130</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4">
+        <v>216760</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1500</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="4">
+        <v>48202</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1875</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added tests suite with pytest
    - test_main.py has been integrated
    - other tests added
    - some improvements to ExcelDB methods
    - removed dependency to xlsxwriter
</commit_message>
<xml_diff>
--- a/test/mountains.xlsx
+++ b/test/mountains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DUO/laurent/Documents/SettleNext2/Div 7 Executive/Development/pythonlib/excel_tables/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E71C417-0572-4248-A674-B79D846D501F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1606E13B-DD2D-744A-9B3D-AC551DF29829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="3160" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="3160" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mountains" sheetId="1" r:id="rId1"/>
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,8 +823,8 @@
         <v>11</v>
       </c>
       <c r="J2">
-        <f ca="1">RAND()</f>
-        <v>0.19565021213661404</v>
+        <f ca="1">ROUND(RAND(), 6)</f>
+        <v>0.109485</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -856,8 +856,8 @@
         <v>17</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J26" ca="1" si="0">RAND()</f>
-        <v>0.22902659152252836</v>
+        <f t="shared" ref="J3:J26" ca="1" si="0">ROUND(RAND(), 6)</f>
+        <v>0.76513200000000003</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -890,7 +890,7 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75612862889360799</v>
+        <v>0.304068</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -923,7 +923,7 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42831088973332443</v>
+        <v>0.52342100000000003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -956,7 +956,7 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31605855813917683</v>
+        <v>0.39655699999999999</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3402207363452727E-2</v>
+        <v>0.273592</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1022,7 +1022,7 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8678175358278128E-2</v>
+        <v>0.268625</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16100919167868266</v>
+        <v>1.7357000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80138352786999589</v>
+        <v>0.18808</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3876381818585598</v>
+        <v>0.88986600000000005</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26427147293054054</v>
+        <v>0.84389800000000004</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1186,8 +1186,8 @@
         <v>17</v>
       </c>
       <c r="J13">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.26539115703915483</v>
+        <f ca="1">ROUND(RAND(), 4)</f>
+        <v>0.309</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72355580947484599</v>
+        <v>0.29202400000000001</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81626279635791466</v>
+        <v>0.47705999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4373928917187988</v>
+        <v>0.87826199999999999</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1319,7 +1319,7 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74774394311773607</v>
+        <v>0.806481</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1352,7 +1352,7 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43407772494803953</v>
+        <v>0.230078</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1385,7 +1385,7 @@
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1832803466713171</v>
+        <v>4.8044000000000003E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1418,7 +1418,7 @@
       </c>
       <c r="J20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6294085854430137</v>
+        <v>0.106818</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="J21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66240744232541227</v>
+        <v>0.647976</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1484,7 +1484,7 @@
       </c>
       <c r="J22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23757369634898351</v>
+        <v>0.61989000000000005</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="J23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41009419459910623</v>
+        <v>0.86195200000000005</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="J24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44959853766447178</v>
+        <v>0.91941099999999998</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="J25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26400432961866915</v>
+        <v>0.59091300000000002</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="J26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28256090673261036</v>
+        <v>0.183695</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +1633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2179DB8B-1E4D-784B-BA8E-3931701E4811}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>

</xml_diff>